<commit_message>
Now supports Low, Hi, and HIHI alarm limits.
</commit_message>
<xml_diff>
--- a/das_facts/template_DasFacts.xlsx
+++ b/das_facts/template_DasFacts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgambrell\Desktop\Generated_Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgambrell\Desktop\code\python\CEMDAS_Tools\das_facts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA9C313-151D-44E0-929E-98CBC5FAC9D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC311F8-5960-4060-AE1C-470DD65F0C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="1890" xr2:uid="{F79795B5-C0A2-4894-A5A4-6AD66AE42B76}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Param_Index</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Data Source</t>
+  </si>
+  <si>
+    <t>Low Limit</t>
+  </si>
+  <si>
+    <t>Hi Limit</t>
+  </si>
+  <si>
+    <t>Hi_Hi Limit</t>
   </si>
 </sst>
 </file>
@@ -454,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0A7825-3EB4-4E1C-9331-6F27A8FB24C6}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +481,7 @@
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,6 +511,15 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now supports "Units", the measure of params.
</commit_message>
<xml_diff>
--- a/das_facts/template_DasFacts.xlsx
+++ b/das_facts/template_DasFacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgambrell\Desktop\code\python\CEMDAS_Tools\das_facts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC311F8-5960-4060-AE1C-470DD65F0C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BEDD4A-B613-4334-A807-8B8F74981514}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="1890" xr2:uid="{F79795B5-C0A2-4894-A5A4-6AD66AE42B76}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Param_Index</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Hi_Hi Limit</t>
+  </si>
+  <si>
+    <t>Units</t>
   </si>
 </sst>
 </file>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0A7825-3EB4-4E1C-9331-6F27A8FB24C6}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +484,7 @@
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,36 +492,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>